<commit_message>
improvements on combined program
</commit_message>
<xml_diff>
--- a/allFunctional/input/IDH_PLC_Tags.xlsx
+++ b/allFunctional/input/IDH_PLC_Tags.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/georgesgregoire/Documents/Code/Omron-AB-Converter/tag_builder/Input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/georgesgregoire/Documents/Code/Python/Omron-AB-Converter/allFunctional/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DFFEC42-1F03-B045-B102-4B3C75709D07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14CDD186-29FF-114F-9836-8C202A89F1E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="49760" yWindow="500" windowWidth="25240" windowHeight="18460" activeTab="1" xr2:uid="{16D0EB3E-8CAD-2C40-A306-CE4D11FA5839}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{16D0EB3E-8CAD-2C40-A306-CE4D11FA5839}"/>
   </bookViews>
   <sheets>
     <sheet name="IO_Cards" sheetId="2" r:id="rId1"/>
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5293" uniqueCount="2275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5294" uniqueCount="2275">
   <si>
     <t>BOOL</t>
   </si>
@@ -7158,11 +7158,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF9C5700"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -7198,11 +7198,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -7921,8 +7921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6609C921-A216-814E-BE32-7DEB6C535032}">
   <dimension ref="A1:D146"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8476,6 +8476,9 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>222</v>
+      </c>
       <c r="B47" t="s">
         <v>1</v>
       </c>
@@ -9616,7 +9619,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C146">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -18513,7 +18516,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C297">
-    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -22051,7 +22054,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B184 C2:C482">
-    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -24410,7 +24413,7 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="B3:B111">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -29122,7 +29125,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:G181">
-    <cfRule type="duplicateValues" dxfId="2" priority="40"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="40"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -29349,7 +29352,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:B15">
-    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>